<commit_message>
Pruebas de API petStore con Swagger parser y RestAssured - MEF
</commit_message>
<xml_diff>
--- a/src/test/resources/datos_petstore.xlsx
+++ b/src/test/resources/datos_petstore.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>NumeroCaso</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>available</t>
+  </si>
+  <si>
+    <t>Caso2</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -401,13 +407,25 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>

</xml_diff>